<commit_message>
enable data extraction of different studies, using setting study_name in compose
</commit_message>
<xml_diff>
--- a/src/obds_fhir_to_opal/output/PoC/data_dictionary_df.xlsx
+++ b/src/obds_fhir_to_opal/output/PoC/data_dictionary_df.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>table</t>
   </si>
@@ -62,74 +62,78 @@
     <t>condition_id</t>
   </si>
   <si>
+    <t>icd10_code</t>
+  </si>
+  <si>
+    <t>icd10_mapped</t>
+  </si>
+  <si>
+    <t>icd10_grouped</t>
+  </si>
+  <si>
+    <t>icd10_entity</t>
+  </si>
+  <si>
     <t>date_diagnosis</t>
   </si>
   <si>
-    <t>icd10_code</t>
+    <t>date_diagnosis_year</t>
+  </si>
+  <si>
+    <t>date_diagnosis_month</t>
+  </si>
+  <si>
+    <t>date_diagnosis_day</t>
   </si>
   <si>
     <t>gender</t>
   </si>
   <si>
-    <t>date_diagnosis_year</t>
-  </si>
-  <si>
-    <t>date_diagnosis_month</t>
-  </si>
-  <si>
-    <t>date_diagnosis_day</t>
-  </si>
-  <si>
-    <t>icd10_mapped</t>
-  </si>
-  <si>
-    <t>icd10_grouped_entities</t>
-  </si>
-  <si>
     <t>gender_mapped</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
+    <t>decimal</t>
+  </si>
+  <si>
     <t>integer</t>
   </si>
   <si>
-    <t>decimal</t>
-  </si>
-  <si>
     <t>Participant</t>
   </si>
   <si>
     <t>Condition ID, unique for each condition</t>
   </si>
   <si>
-    <t>date of diagnosis</t>
-  </si>
-  <si>
     <t>ICD10 GM diagnosis code</t>
-  </si>
-  <si>
-    <t>Gender - male, female, other/diverse</t>
-  </si>
-  <si>
-    <t>Year of Diagnosis</t>
-  </si>
-  <si>
-    <t>Month of Diagnosis</t>
-  </si>
-  <si>
-    <t>Day of Diagnosis</t>
   </si>
   <si>
     <t>ICD10 GM diagnosis code mapped A = 1, B = 2, C = 3, D = 4,
         e.g.: A01.9 = 101.9, C50.1 = 350.1 or D41.9 = 441.9</t>
   </si>
   <si>
-    <t>ICD10 GM diagnosis code grouped to entity groups
-        from 0-23 according to LGL Report Cancer in Bavaria 2019, mapping see
-        github.com/bzkf/onco-analytics-on-fhir/src/obds_fhir_to_opal
-        /utils_onco_analytics.py</t>
+    <t>ICD10 GM diagnosis code grouped to parent code, e.g. A01.1
+        and A01.9 both belong to group 101 (remove decimal from icd10_mapped)</t>
+  </si>
+  <si>
+    <t>Entities of resulting ICD10 groups, see utils</t>
+  </si>
+  <si>
+    <t>Date of diagnosis</t>
+  </si>
+  <si>
+    <t>Year of diagnosis</t>
+  </si>
+  <si>
+    <t>Month of Diagnosis</t>
+  </si>
+  <si>
+    <t>Day of Diagnosis</t>
+  </si>
+  <si>
+    <t>Gender - male, female, other/diverse</t>
   </si>
   <si>
     <t>Gender mapped: 0 = None, 1 = female, 2 = male,
@@ -500,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -555,10 +559,10 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -567,7 +571,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -578,10 +582,10 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -590,7 +594,7 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -601,10 +605,10 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -613,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -624,10 +628,10 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -636,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -647,10 +651,10 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -659,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -673,7 +677,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -682,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -693,10 +697,10 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -705,7 +709,7 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -716,10 +720,10 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -728,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -739,10 +743,10 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -751,7 +755,7 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -765,16 +769,39 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="L11" t="s">
-        <v>37</v>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -795,16 +822,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work in very big progress
</commit_message>
<xml_diff>
--- a/src/obds_fhir_to_opal/output/PoC/data_dictionary_df.xlsx
+++ b/src/obds_fhir_to_opal/output/PoC/data_dictionary_df.xlsx
@@ -110,34 +110,31 @@
     <t>ICD10 GM diagnosis code</t>
   </si>
   <si>
-    <t>ICD10 GM diagnosis code mapped A = 1, B = 2, C = 3, D = 4,
-        e.g.: A01.9 = 101.9, C50.1 = 350.1 or D41.9 = 441.9</t>
-  </si>
-  <si>
-    <t>ICD10 GM diagnosis code grouped to parent code, e.g. A01.1
-        and A01.9 both belong to group 101 (remove decimal from icd10_mapped)</t>
-  </si>
-  <si>
-    <t>Entities of resulting ICD10 groups, see utils</t>
-  </si>
-  <si>
-    <t>Date of diagnosis</t>
+    <t>ICD10 GM diagnosis code mapped A = 1, B = 2, C = 3, D = 4, e.g.: A01.9 = 101.9, C50.1 = 350.1 or D41.9 = 441.9</t>
+  </si>
+  <si>
+    <t>ICD10 GM diagnosis code grouped to parent code, e.g. A01.1 and A01.9 both belong to group 101 (remove decimal from icd10_mapped)</t>
+  </si>
+  <si>
+    <t>ICD10 GM diagnosis code grouped to entity groups from 0-23 according to LGL Report Cancer in Bavaria 2019, mapping see github.com/bzkf/onco-analytics-on-fhir/src/obds_fhir_to_opal/utils_onco_analytics.py</t>
+  </si>
+  <si>
+    <t>date of diagnosis</t>
   </si>
   <si>
     <t>Year of diagnosis</t>
   </si>
   <si>
-    <t>Month of Diagnosis</t>
-  </si>
-  <si>
-    <t>Day of Diagnosis</t>
+    <t>Month of diagnosis</t>
+  </si>
+  <si>
+    <t>Day of diagnosis</t>
   </si>
   <si>
     <t>Gender - male, female, other/diverse</t>
   </si>
   <si>
-    <t>Gender mapped: 0 = None, 1 = female, 2 = male,
-        3 = other/diverse</t>
+    <t>Gender mapped: 0 = None, 1 = female, 2 = male, 3 = other/diverse</t>
   </si>
   <si>
     <t>variable</t>

</xml_diff>